<commit_message>
Added more email functionality
</commit_message>
<xml_diff>
--- a/boost/smuckers/resources/boltemplate.xlsx
+++ b/boost/smuckers/resources/boltemplate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t xml:space="preserve">(Uniform Domestic Straight Bill of Lading adopted by Carriers in Official, Southern, Western and Illinois </t>
   </si>
@@ -232,9 +232,6 @@
   </si>
   <si>
     <t>Per</t>
-  </si>
-  <si>
-    <t>(This is where the truck drivers name will go)</t>
   </si>
   <si>
     <t xml:space="preserve">Permanent post office </t>
@@ -611,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -765,7 +762,6 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
@@ -968,7 +964,7 @@
       <c r="P11" s="12"/>
       <c r="Q11" s="18">
         <f>NOW()</f>
-        <v>42936.80173</v>
+        <v>42949.46595</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
@@ -1741,14 +1737,12 @@
         <v>58</v>
       </c>
       <c r="K53" s="16"/>
-      <c r="L53" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="M53" s="16"/>
-      <c r="N53" s="79"/>
-      <c r="O53" s="79"/>
-      <c r="P53" s="79"/>
-      <c r="Q53" s="79"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
     </row>
     <row r="54" ht="12.0" customHeight="1">
       <c r="A54" s="4"/>
@@ -1770,11 +1764,11 @@
       <c r="Q54" s="7"/>
     </row>
     <row r="55" ht="12.0" customHeight="1">
-      <c r="A55" s="80" t="s">
+      <c r="A55" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="E55" s="80" t="s">
         <v>60</v>
-      </c>
-      <c r="E55" s="81" t="s">
-        <v>61</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="19"/>
@@ -1786,15 +1780,15 @@
       <c r="Q55" s="10"/>
     </row>
     <row r="56" ht="9.75" customHeight="1">
-      <c r="A56" s="80" t="s">
-        <v>62</v>
+      <c r="A56" s="79" t="s">
+        <v>61</v>
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
-      <c r="J56" s="82"/>
+      <c r="J56" s="81"/>
       <c r="K56" s="19"/>
       <c r="L56" s="19"/>
       <c r="M56" s="19"/>
@@ -1808,13 +1802,13 @@
       <c r="B57" s="19"/>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
-      <c r="E57" s="83" t="s">
-        <v>63</v>
+      <c r="E57" s="82" t="s">
+        <v>62</v>
       </c>
-      <c r="F57" s="84"/>
-      <c r="G57" s="84"/>
-      <c r="H57" s="84"/>
-      <c r="I57" s="84"/>
+      <c r="F57" s="83"/>
+      <c r="G57" s="83"/>
+      <c r="H57" s="83"/>
+      <c r="I57" s="83"/>
       <c r="J57" s="19"/>
       <c r="K57" s="19"/>
       <c r="L57" s="19"/>
@@ -19742,107 +19736,108 @@
       <c r="Q1000" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="100">
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="P7:Q7"/>
+  <mergeCells count="101">
+    <mergeCell ref="A18:Q18"/>
+    <mergeCell ref="A14:Q17"/>
+    <mergeCell ref="A4:Q4"/>
     <mergeCell ref="L5:P5"/>
+    <mergeCell ref="D19:P19"/>
     <mergeCell ref="A9:Q9"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A3:Q3"/>
-    <mergeCell ref="A4:Q4"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="C13:P13"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:Q28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="C38:H38"/>
     <mergeCell ref="C39:H39"/>
     <mergeCell ref="C37:H37"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
     <mergeCell ref="E55:I56"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A55:D55"/>
     <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="K36:L36"/>
     <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M37:N37"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="K38:L38"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="M38:N38"/>
     <mergeCell ref="I39:J39"/>
     <mergeCell ref="I38:J38"/>
     <mergeCell ref="M39:N39"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="O37:Q37"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O39:Q39"/>
     <mergeCell ref="O42:Q42"/>
-    <mergeCell ref="O39:Q39"/>
     <mergeCell ref="O40:Q40"/>
     <mergeCell ref="O41:Q41"/>
-    <mergeCell ref="O38:Q38"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K53:Q53"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="A3:Q3"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="O33:Q35"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="O32:Q32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
     <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="O33:Q35"/>
-    <mergeCell ref="O32:Q32"/>
-    <mergeCell ref="O37:Q37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="A14:Q17"/>
-    <mergeCell ref="O27:Q28"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="C13:P13"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="A18:Q18"/>
-    <mergeCell ref="D19:P19"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>